<commit_message>
added Movable object to maps, task list updated
</commit_message>
<xml_diff>
--- a/Task List - Edit.xlsx
+++ b/Task List - Edit.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\Visual Studio 2013\Projects\Studio Project 1 -test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsy00\Desktop\SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="280" yWindow="550" windowWidth="24610" windowHeight="14260"/>
+    <workbookView xWindow="276" yWindow="552" windowWidth="24612" windowHeight="14256"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Task List - Preview / Review</t>
   </si>
@@ -142,15 +142,9 @@
     <t>SY</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Transitions between maps</t>
   </si>
   <si>
-    <t>Interactive objects</t>
-  </si>
-  <si>
     <t>Control edits</t>
   </si>
   <si>
@@ -164,12 +158,27 @@
   </si>
   <si>
     <t>Map(level designs, i, )</t>
+  </si>
+  <si>
+    <t>Movable objects</t>
+  </si>
+  <si>
+    <t>Victory screen</t>
+  </si>
+  <si>
+    <t>Splashscreen</t>
+  </si>
+  <si>
+    <t>Chest and key</t>
+  </si>
+  <si>
+    <t>Doors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -485,30 +494,60 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -535,36 +574,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,6 +781,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -851,6 +908,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -886,6 +960,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1064,36 +1155,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.90625" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="39.54296875" customWidth="1"/>
-    <col min="4" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="7" width="5.36328125" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" customWidth="1"/>
-    <col min="10" max="10" width="32.453125" customWidth="1"/>
-    <col min="11" max="11" width="0.90625" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" customWidth="1"/>
+    <col min="4" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="32.44140625" customWidth="1"/>
+    <col min="11" max="11" width="0.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.5">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:11" ht="17.399999999999999">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
@@ -1110,10 +1201,10 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="4">
         <v>1</v>
       </c>
@@ -1125,20 +1216,20 @@
         <v>3</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="35"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1147,22 +1238,22 @@
       </c>
       <c r="E4" s="8">
         <f>SUMIF(D$10:D27, D4, E$10:E27)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="41"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="16" t="s">
         <v>22</v>
       </c>
@@ -1171,22 +1262,22 @@
       </c>
       <c r="E5" s="9">
         <f>SUMIF(D$10:D27, D5, E$10:E27)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="41"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
@@ -1195,22 +1286,22 @@
       </c>
       <c r="E6" s="9">
         <f>SUMIF(D$10:D27, D6, E$10:E27)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
@@ -1219,14 +1310,14 @@
       </c>
       <c r="E7" s="9">
         <f>SUMIF(D$10:D27, D7, E$10:E27)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="42"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="15" t="s">
         <v>13</v>
       </c>
@@ -1249,10 +1340,10 @@
       <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="12" t="s">
         <v>16</v>
       </c>
@@ -1262,114 +1353,114 @@
       <c r="F9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="18"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="18"/>
+      <c r="B10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="20"/>
       <c r="D10" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="9">
         <v>15</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="18"/>
+      <c r="F10" s="9">
+        <v>20</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="9">
         <v>2</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="18"/>
+      <c r="B11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="20"/>
       <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="9">
         <v>3</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="18"/>
+      <c r="F11" s="9">
+        <v>4</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="9">
         <v>3</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="18"/>
+      <c r="B12" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="20"/>
       <c r="D12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="9">
         <v>4</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="18"/>
+      <c r="F12" s="9">
+        <v>5</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="20"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="9">
         <v>4</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="18"/>
+      <c r="B13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="20"/>
       <c r="D13" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F13" s="9">
-        <v>1</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="18"/>
+      <c r="B14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="20"/>
       <c r="D14" s="9" t="s">
         <v>27</v>
       </c>
@@ -1379,206 +1470,246 @@
       <c r="F14" s="9">
         <v>2</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="18"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="9">
         <v>6</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="18"/>
+      <c r="B15" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="20"/>
       <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="9">
         <v>15</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="18"/>
+      <c r="F15" s="9">
+        <v>10</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="9">
         <v>7</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="18"/>
+      <c r="B16" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="20"/>
       <c r="D16" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" s="9">
         <v>4</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="18"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="18"/>
+      <c r="A17" s="9">
+        <v>8</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="9">
+        <v>4</v>
+      </c>
+      <c r="F17" s="9">
+        <v>6</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="18"/>
+      <c r="A18" s="9">
+        <v>9</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="18"/>
+      <c r="A19" s="9">
+        <v>10</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="18"/>
+      <c r="A20" s="9">
+        <v>11</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="9">
+        <v>3</v>
+      </c>
+      <c r="F20" s="9">
+        <v>3</v>
+      </c>
+      <c r="G20" s="23"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1">
       <c r="A21" s="9"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="18"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1">
       <c r="A22" s="9"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="18"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
       <c r="A23" s="9"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="18"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="A24" s="9"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="18"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="A25" s="9"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="18"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="A26" s="9"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="18"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
       <c r="A27" s="9"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="18"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="18"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9">
         <f>SUM(E10:E27)</f>
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="F28" s="9">
         <f>SUM(F10:F27)</f>
-        <v>7</v>
-      </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="18"/>
+        <v>61</v>
+      </c>
+      <c r="G28" s="23"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
       <c r="A29" s="3"/>
@@ -1593,11 +1724,11 @@
       <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="18"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1607,42 +1738,42 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="37"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="30"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="40"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="33"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="43"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34" s="3"/>
@@ -1669,34 +1800,34 @@
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A37" s="19" t="str">
+      <c r="A37" s="34" t="str">
         <f>C4</f>
         <v>Alan Koh Song Hua</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="19" t="str">
+      <c r="E37" s="34" t="str">
         <f>C5</f>
         <v>Darryl Peter s/o Jeret</v>
       </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38" s="3"/>
@@ -1710,35 +1841,35 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="12.5">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+    <row r="39" spans="1:10" ht="13.2">
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-    </row>
-    <row r="40" spans="1:10" ht="12.5">
-      <c r="A40" s="19" t="str">
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+    </row>
+    <row r="40" spans="1:10" ht="13.2">
+      <c r="A40" s="34" t="str">
         <f>C6</f>
         <v>Chan Wen Hao Ryan</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="19" t="str">
+      <c r="E40" s="34" t="str">
         <f>C7</f>
         <v>Heng Sheng Yang</v>
       </c>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1">
       <c r="A41" s="3"/>
@@ -1754,6 +1885,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="A31:J33"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="H3:I3"/>
@@ -1770,48 +1943,6 @@
     <mergeCell ref="A4:B7"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="A31:J33"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more signs, and edited some texts
</commit_message>
<xml_diff>
--- a/Task List - Edit.xlsx
+++ b/Task List - Edit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Studio Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\Visual Studio 2013\Projects\Studio Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -175,9 +175,6 @@
     <t>Doors</t>
   </si>
   <si>
-    <t>Torchlight</t>
-  </si>
-  <si>
     <t>Mainmenu</t>
   </si>
   <si>
@@ -188,12 +185,15 @@
   </si>
   <si>
     <t>Background music</t>
+  </si>
+  <si>
+    <t>Fog of war</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -509,30 +509,60 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -559,36 +589,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,6 +892,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -971,23 +1019,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1023,23 +1054,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1219,7 +1233,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1236,7 +1250,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18"/>
@@ -1267,7 +1281,7 @@
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="4">
         <v>1</v>
       </c>
@@ -1279,20 +1293,20 @@
         <v>3</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="38"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1305,18 +1319,18 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="43"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="16" t="s">
         <v>22</v>
       </c>
@@ -1329,18 +1343,18 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="43"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
@@ -1353,18 +1367,18 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
@@ -1377,10 +1391,10 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="35"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="15" t="s">
         <v>13</v>
       </c>
@@ -1403,10 +1417,10 @@
       <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="12" t="s">
         <v>16</v>
       </c>
@@ -1416,22 +1430,22 @@
       <c r="F9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="9" t="s">
         <v>28</v>
       </c>
@@ -1441,20 +1455,20 @@
       <c r="F10" s="9">
         <v>20</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="9">
         <v>2</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="9" t="s">
         <v>25</v>
       </c>
@@ -1464,20 +1478,20 @@
       <c r="F11" s="9">
         <v>4</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="21"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="9">
         <v>3</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="9" t="s">
         <v>26</v>
       </c>
@@ -1487,20 +1501,20 @@
       <c r="F12" s="9">
         <v>5</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="20"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="9">
         <v>4</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="9" t="s">
         <v>27</v>
       </c>
@@ -1510,20 +1524,20 @@
       <c r="F13" s="9">
         <v>5</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="9">
         <v>5</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="9" t="s">
         <v>27</v>
       </c>
@@ -1533,19 +1547,19 @@
       <c r="F14" s="9">
         <v>2</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="9">
         <v>6</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
@@ -1555,19 +1569,19 @@
       <c r="F15" s="9">
         <v>10</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="9">
         <v>7</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="9" t="s">
         <v>28</v>
       </c>
@@ -1577,19 +1591,19 @@
       <c r="F16" s="9">
         <v>4</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="21"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1">
       <c r="A17" s="9">
         <v>8</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="9" t="s">
         <v>28</v>
       </c>
@@ -1599,19 +1613,19 @@
       <c r="F17" s="9">
         <v>6</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="21"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1">
       <c r="A18" s="9">
         <v>9</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="9" t="s">
         <v>26</v>
       </c>
@@ -1621,19 +1635,19 @@
       <c r="F18" s="9">
         <v>1</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="9">
         <v>10</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="9" t="s">
         <v>27</v>
       </c>
@@ -1643,19 +1657,19 @@
       <c r="F19" s="9">
         <v>1</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="9">
         <v>11</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="21"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="9" t="s">
         <v>25</v>
       </c>
@@ -1665,19 +1679,19 @@
       <c r="F20" s="9">
         <v>3</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1">
       <c r="A21" s="9">
         <v>12</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="21"/>
+      <c r="B21" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="20"/>
       <c r="D21" s="9" t="s">
         <v>28</v>
       </c>
@@ -1687,19 +1701,19 @@
       <c r="F21" s="9">
         <v>3</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1">
       <c r="A22" s="9">
         <v>13</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="21"/>
+      <c r="B22" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="20"/>
       <c r="D22" s="9" t="s">
         <v>28</v>
       </c>
@@ -1709,19 +1723,19 @@
       <c r="F22" s="9">
         <v>3</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
       <c r="A23" s="9">
         <v>14</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="21"/>
+      <c r="B23" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="20"/>
       <c r="D23" s="9" t="s">
         <v>28</v>
       </c>
@@ -1731,19 +1745,19 @@
       <c r="F23" s="9">
         <v>0.5</v>
       </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="A24" s="9">
         <v>15</v>
       </c>
-      <c r="B24" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="21"/>
+      <c r="B24" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="20"/>
       <c r="D24" s="9" t="s">
         <v>26</v>
       </c>
@@ -1753,19 +1767,19 @@
       <c r="F24" s="9">
         <v>2</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="21"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="A25" s="9">
         <v>16</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="21"/>
+      <c r="B25" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="20"/>
       <c r="D25" s="9" t="s">
         <v>27</v>
       </c>
@@ -1775,41 +1789,41 @@
       <c r="F25" s="9">
         <v>2</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="21"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="A26" s="9"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="21"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
       <c r="A27" s="9"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="21"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9">
         <f>SUM(E10:E27)</f>
@@ -1819,10 +1833,10 @@
         <f>SUM(F10:F27)</f>
         <v>71.5</v>
       </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="21"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
       <c r="A29" s="3"/>
@@ -1837,11 +1851,11 @@
       <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1851,42 +1865,42 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="37"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="30"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="40"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="33"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="43"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34" s="3"/>
@@ -1913,26 +1927,26 @@
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A37" s="17" t="str">
+      <c r="A37" s="34" t="str">
         <f>C4</f>
         <v>Alan Koh Song Hua</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="17" t="str">
+      <c r="E37" s="34" t="str">
         <f>C5</f>
         <v>Darryl Peter s/o Jeret</v>
       </c>
@@ -1955,26 +1969,26 @@
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" ht="12.5">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:10" ht="12.5">
-      <c r="A40" s="17" t="str">
+      <c r="A40" s="34" t="str">
         <f>C6</f>
         <v>Chan Wen Hao Ryan</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="17" t="str">
+      <c r="E40" s="34" t="str">
         <f>C7</f>
         <v>Heng Sheng Yang</v>
       </c>
@@ -1998,6 +2012,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="A31:J33"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G15:J15"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="H3:I3"/>
@@ -2014,48 +2070,6 @@
     <mergeCell ref="A4:B7"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="A31:J33"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>